<commit_message>
Add the some initial data for testing purpose
</commit_message>
<xml_diff>
--- a/docs/scripts/Permission.Design.xlsx
+++ b/docs/scripts/Permission.Design.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="149" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="648" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="SAProject" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="view.permissions" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Workitem Status" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Roles" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="SAProject" sheetId="1" r:id="rId1"/>
+    <sheet name="view.permissions" sheetId="2" r:id="rId2"/>
+    <sheet name="Workitem Status" sheetId="3" r:id="rId3"/>
+    <sheet name="Roles" sheetId="4" r:id="rId4"/>
+    <sheet name="Releases" sheetId="5" r:id="rId5"/>
+    <sheet name="WorkItemGroup" sheetId="6" r:id="rId6"/>
+    <sheet name="WorkItem" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="356">
   <si>
     <t>Project Permissions</t>
   </si>
@@ -100,29 +102,29 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">If project was 'PUBLIC', it can be viewd for everyone;
+      <t>If project was 'PUBLIC', it can be viewd for everyone;
 otherwise, it can be only viewd for project members.
 "</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <color rgb="000070C0"/>
-        <sz val="9"/>
       </rPr>
-      <t xml:space="preserve">Work on workitem</t>
+      <t>Work on workitem</t>
     </r>
     <r>
       <rPr>
+        <sz val="9"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <sz val="9"/>
       </rPr>
-      <t xml:space="preserve">" permission should depend on this.</t>
+      <t>" permission should depend on this.</t>
     </r>
   </si>
   <si>
@@ -386,88 +388,88 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <color rgb="000070C0"/>
-        <sz val="9"/>
       </rPr>
-      <t xml:space="preserve">Modify</t>
+      <t>Modify</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF333333"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <color rgb="00333333"/>
-        <sz val="9"/>
       </rPr>
-      <t xml:space="preserve">,</t>
+      <t>,</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <color rgb="000070C0"/>
-        <sz val="9"/>
       </rPr>
       <t xml:space="preserve"> Schedule</t>
     </r>
     <r>
       <rPr>
+        <sz val="9"/>
+        <color rgb="FF333333"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <color rgb="00333333"/>
-        <sz val="9"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <color rgb="000070C0"/>
-        <sz val="9"/>
       </rPr>
-      <t xml:space="preserve">Include</t>
+      <t>Include</t>
     </r>
     <r>
       <rPr>
+        <sz val="9"/>
+        <color rgb="FF333333"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <color rgb="00333333"/>
-        <sz val="9"/>
       </rPr>
       <t xml:space="preserve"> and </t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <color rgb="000070C0"/>
-        <sz val="9"/>
       </rPr>
-      <t xml:space="preserve">Exclude</t>
+      <t>Exclude</t>
     </r>
     <r>
       <rPr>
+        <sz val="9"/>
+        <color rgb="FF333333"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <color rgb="00333333"/>
-        <sz val="9"/>
       </rPr>
-      <t xml:space="preserve">.</t>
+      <t>.</t>
     </r>
   </si>
   <si>
@@ -559,28 +561,28 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Permission to assign this workitem to somebody (who should be has the permission of</t>
+      <t>Permission to assign this workitem to somebody (who should be has the permission of</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <color rgb="000070C0"/>
-        <sz val="9"/>
       </rPr>
       <t xml:space="preserve"> Assignable User</t>
     </r>
     <r>
       <rPr>
+        <sz val="9"/>
+        <color rgb="FF333333"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <color rgb="00333333"/>
-        <sz val="9"/>
       </rPr>
-      <t xml:space="preserve">.</t>
+      <t>.</t>
     </r>
   </si>
   <si>
@@ -598,23 +600,23 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <color rgb="000070C0"/>
-        <sz val="9"/>
       </rPr>
-      <t xml:space="preserve">Assign Workitem</t>
+      <t>Assign Workitem</t>
     </r>
     <r>
       <rPr>
+        <sz val="9"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <sz val="9"/>
       </rPr>
-      <t xml:space="preserve">.</t>
+      <t>.</t>
     </r>
   </si>
   <si>
@@ -1139,223 +1141,334 @@
   </si>
   <si>
     <t>Stuff User, Has the permission to access System Administartion Page.</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>project_id</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>deadline</t>
+  </si>
+  <si>
+    <t>update_time</t>
+  </si>
+  <si>
+    <t>last_edited_by</t>
+  </si>
+  <si>
+    <t>v01.00.00</t>
+  </si>
+  <si>
+    <t>v01.00.00 release notes</t>
+  </si>
+  <si>
+    <t>userpo</t>
+  </si>
+  <si>
+    <t>v01.01.00</t>
+  </si>
+  <si>
+    <t>v01.01.00 release notes</t>
+  </si>
+  <si>
+    <t>v02.00.00</t>
+  </si>
+  <si>
+    <t>v02.00.00 release notes</t>
+  </si>
+  <si>
+    <t>2013-09-30</t>
+  </si>
+  <si>
+    <t>2013-12-31</t>
+  </si>
+  <si>
+    <t>2014-04-30</t>
+  </si>
+  <si>
+    <t>parent_id</t>
+  </si>
+  <si>
+    <t>importance</t>
+  </si>
+  <si>
+    <t>time_logged</t>
+  </si>
+  <si>
+    <t>initial_estimate</t>
+  </si>
+  <si>
+    <t>Login Interface</t>
+  </si>
+  <si>
+    <t>Implement the Login functions for the site</t>
+  </si>
+  <si>
+    <t>Project Tree display</t>
+  </si>
+  <si>
+    <t>We need a tree display diagram for the projects own by one user</t>
+  </si>
+  <si>
+    <t>Project Edit/Add</t>
+  </si>
+  <si>
+    <t>Project creation and edition function for specific project</t>
+  </si>
+  <si>
+    <t>work_item_group_id</t>
+  </si>
+  <si>
+    <t>release_id</t>
+  </si>
+  <si>
+    <t>loe</t>
+  </si>
+  <si>
+    <t>creator_id</t>
+  </si>
+  <si>
+    <t>assignee_id</t>
+  </si>
+  <si>
+    <t>requestor_id</t>
+  </si>
+  <si>
+    <t>Create Login View</t>
+  </si>
+  <si>
+    <t>Create Login View description</t>
+  </si>
+  <si>
+    <t>Create Login Pagelet</t>
+  </si>
+  <si>
+    <t>Create Login Pagelet description</t>
+  </si>
+  <si>
+    <t>Redirect Login</t>
+  </si>
+  <si>
+    <t>Redirect Login description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="宋体"/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00333333"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="宋体"/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00333333"/>
-      <sz val="8"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF0070C0"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00333333"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="宋体"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00333333"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <sz val="8"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="8"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FFBFBFBF"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="000070C0"/>
-      <sz val="9"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <sz val="8"/>
+      <color rgb="FFBFBFBF"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="9"/>
     </font>
     <font>
-      <name val="宋体"/>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00BFBFBF"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="宋体"/>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00BFBFBF"/>
-      <sz val="8"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="宋体"/>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="8"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FFA6A6A6"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00333333"/>
-      <sz val="9"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <sz val="8"/>
+      <color rgb="FFA6A6A6"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00333333"/>
-      <sz val="9"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="3"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="3"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00A6A6A6"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="宋体"/>
+      <sz val="8"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="3"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00A6A6A6"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="DejaVu Sans Mono"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="3"/>
-      <color rgb="00333333"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="DejaVu Sans Mono"/>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="3"/>
-      <color rgb="00000000"/>
-      <sz val="8"/>
     </font>
     <font>
-      <name val="DejaVu Sans Mono"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="3"/>
-      <sz val="8"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="9"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="9"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1367,314 +1480,292 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F0F0F0"/>
-        <bgColor rgb="00FFFFFF"/>
+        <fgColor rgb="FFF0F0F0"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-        <bgColor rgb="00F0F0F0"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFF0F0F0"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="6">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </left>
       <right style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </right>
       <top style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </top>
       <bottom style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </right>
       <top style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </top>
       <bottom style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </right>
       <top style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </left>
       <right style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </right>
       <top style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="thick">
-        <color rgb="00DDDDDD"/>
+        <color rgb="FFDDDDDD"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="8" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="10" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="10" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="13" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="13" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="10" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="3" fontId="10" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="3" fontId="14" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="3" fontId="15" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="3" fontId="15" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="16" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="17" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="17" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="10" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="14" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="15" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="15" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="20" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="14" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="21" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="22" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="22" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="23" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="23" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="23" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="24" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="24" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="13" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="25" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="25" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="24" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="26" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="27" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="26" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="26" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="26" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="26" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="26" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="28" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="29" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="29" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="26" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="26" numFmtId="164" xfId="0"/>
+  <cellXfs count="75">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1733,13 +1824,21 @@
       <rgbColor rgb="00993366"/>
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1755,11 +1854,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="" id="0" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1779,28 +1878,309 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A2:F90"/>
+  <dimension ref="A2:AMK90"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100">
-      <selection activeCell="D2" activeCellId="0" pane="topLeft" sqref="B2:D73"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D2" sqref="B2:D73"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.3882352941176"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="32.3843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="85.0745098039216"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="29.2156862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="25.9725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="65.0901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="5" width="9.22352941176471"/>
+    <col min="1" max="1" width="24.375" style="1"/>
+    <col min="2" max="2" width="32.375" style="2"/>
+    <col min="3" max="3" width="85.125" style="2"/>
+    <col min="4" max="4" width="29.25" style="3"/>
+    <col min="5" max="5" width="26" style="4"/>
+    <col min="6" max="6" width="65.125" style="1"/>
+    <col min="7" max="1025" width="9.25" style="5"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="2">
+    <row r="2" spans="1:6" ht="10.15" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1820,7 +2200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="3">
+    <row r="3" spans="1:6" ht="10.15" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
@@ -1838,7 +2218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="4">
+    <row r="4" spans="1:6" ht="10.15" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
@@ -1856,7 +2236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="5">
+    <row r="5" spans="1:6" ht="10.15" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
@@ -1874,7 +2254,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="6">
+    <row r="6" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
@@ -1892,7 +2272,7 @@
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="29.85" outlineLevel="0" r="7">
+    <row r="7" spans="1:6" ht="29.85" customHeight="1">
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
@@ -1910,7 +2290,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="8">
+    <row r="8" spans="1:6" ht="10.15" customHeight="1">
       <c r="A8" s="13" t="s">
         <v>27</v>
       </c>
@@ -1928,7 +2308,7 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="9">
+    <row r="9" spans="1:6" ht="10.15" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>31</v>
       </c>
@@ -1946,7 +2326,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="10">
+    <row r="10" spans="1:6" ht="10.15" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>34</v>
       </c>
@@ -1964,7 +2344,7 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="11" s="25">
+    <row r="11" spans="1:6" s="25" customFormat="1" ht="10.15" customHeight="1">
       <c r="A11" s="20" t="s">
         <v>37</v>
       </c>
@@ -1982,7 +2362,7 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="12" s="29">
+    <row r="12" spans="1:6" s="29" customFormat="1" ht="10.15" customHeight="1">
       <c r="A12" s="26" t="s">
         <v>41</v>
       </c>
@@ -1994,7 +2374,7 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="13">
+    <row r="13" spans="1:6" ht="10.15" customHeight="1">
       <c r="A13" s="13" t="s">
         <v>43</v>
       </c>
@@ -2014,7 +2394,7 @@
         <v>47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="14">
+    <row r="14" spans="1:6" ht="10.15" customHeight="1">
       <c r="A14" s="30" t="s">
         <v>48</v>
       </c>
@@ -2024,7 +2404,7 @@
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="15">
+    <row r="15" spans="1:6" ht="10.15" customHeight="1">
       <c r="A15" s="13" t="s">
         <v>49</v>
       </c>
@@ -2044,7 +2424,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="16">
+    <row r="16" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>53</v>
       </c>
@@ -2062,7 +2442,7 @@
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="17">
+    <row r="17" spans="1:6" ht="10.15" customHeight="1">
       <c r="A17" s="13" t="s">
         <v>58</v>
       </c>
@@ -2080,7 +2460,7 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="18">
+    <row r="18" spans="1:6" ht="10.15" customHeight="1">
       <c r="A18" s="13" t="s">
         <v>61</v>
       </c>
@@ -2098,7 +2478,7 @@
         <v>65</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="19">
+    <row r="19" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A19" s="13" t="s">
         <v>66</v>
       </c>
@@ -2116,7 +2496,7 @@
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="20">
+    <row r="20" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A20" s="13" t="s">
         <v>69</v>
       </c>
@@ -2134,7 +2514,7 @@
         <v>71</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="21">
+    <row r="21" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A21" s="13" t="s">
         <v>72</v>
       </c>
@@ -2152,7 +2532,7 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="22">
+    <row r="22" spans="1:6" ht="10.15" customHeight="1">
       <c r="A22" s="13" t="s">
         <v>75</v>
       </c>
@@ -2170,7 +2550,7 @@
         <v>78</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="23">
+    <row r="23" spans="1:6" ht="10.15" customHeight="1">
       <c r="A23" s="13" t="s">
         <v>79</v>
       </c>
@@ -2188,7 +2568,7 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="24">
+    <row r="24" spans="1:6" ht="10.15" customHeight="1">
       <c r="A24" s="13" t="s">
         <v>82</v>
       </c>
@@ -2206,7 +2586,7 @@
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="25">
+    <row r="25" spans="1:6" ht="10.15" customHeight="1">
       <c r="A25" s="13" t="s">
         <v>86</v>
       </c>
@@ -2224,7 +2604,7 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="26">
+    <row r="26" spans="1:6" ht="10.15" customHeight="1">
       <c r="A26" s="30" t="s">
         <v>89</v>
       </c>
@@ -2234,7 +2614,7 @@
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="27">
+    <row r="27" spans="1:6" ht="10.15" customHeight="1">
       <c r="A27" s="13" t="s">
         <v>90</v>
       </c>
@@ -2254,7 +2634,7 @@
         <v>93</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="28">
+    <row r="28" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A28" s="13" t="s">
         <v>94</v>
       </c>
@@ -2272,7 +2652,7 @@
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="29">
+    <row r="29" spans="1:6" ht="10.15" customHeight="1">
       <c r="A29" s="13" t="s">
         <v>98</v>
       </c>
@@ -2290,7 +2670,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="30">
+    <row r="30" spans="1:6" ht="10.15" customHeight="1">
       <c r="A30" s="13" t="s">
         <v>101</v>
       </c>
@@ -2308,7 +2688,7 @@
         <v>103</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="31">
+    <row r="31" spans="1:6" ht="10.15" customHeight="1">
       <c r="A31" s="13" t="s">
         <v>104</v>
       </c>
@@ -2326,7 +2706,7 @@
         <v>107</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20.85" outlineLevel="0" r="32">
+    <row r="32" spans="1:6" ht="20.85" customHeight="1">
       <c r="A32" s="13" t="s">
         <v>108</v>
       </c>
@@ -2344,7 +2724,7 @@
         <v>111</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="33">
+    <row r="33" spans="1:6" ht="10.15" customHeight="1">
       <c r="A33" s="13" t="s">
         <v>112</v>
       </c>
@@ -2362,7 +2742,7 @@
         <v>78</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="34">
+    <row r="34" spans="1:6" ht="10.15" customHeight="1">
       <c r="A34" s="13" t="s">
         <v>115</v>
       </c>
@@ -2380,7 +2760,7 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="35">
+    <row r="35" spans="1:6" ht="10.15" customHeight="1">
       <c r="A35" s="30" t="s">
         <v>117</v>
       </c>
@@ -2390,7 +2770,7 @@
       <c r="E35" s="30"/>
       <c r="F35" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="36">
+    <row r="36" spans="1:6" ht="10.15" customHeight="1">
       <c r="A36" s="33" t="s">
         <v>118</v>
       </c>
@@ -2408,7 +2788,7 @@
       </c>
       <c r="F36" s="33"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="37">
+    <row r="37" spans="1:6" ht="10.15" customHeight="1">
       <c r="A37" s="13" t="s">
         <v>121</v>
       </c>
@@ -2426,7 +2806,7 @@
         <v>124</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="38">
+    <row r="38" spans="1:6" ht="10.15" customHeight="1">
       <c r="A38" s="13" t="s">
         <v>125</v>
       </c>
@@ -2444,7 +2824,7 @@
         <v>127</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="39">
+    <row r="39" spans="1:6" ht="10.15" customHeight="1">
       <c r="A39" s="13" t="s">
         <v>128</v>
       </c>
@@ -2462,7 +2842,7 @@
         <v>131</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="40">
+    <row r="40" spans="1:6" ht="10.15" customHeight="1">
       <c r="A40" s="13" t="s">
         <v>132</v>
       </c>
@@ -2480,7 +2860,7 @@
         <v>136</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="11.3" outlineLevel="0" r="41">
+    <row r="41" spans="1:6" ht="11.25" customHeight="1">
       <c r="A41" s="13" t="s">
         <v>137</v>
       </c>
@@ -2498,7 +2878,7 @@
         <v>141</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="11.3" outlineLevel="0" r="42">
+    <row r="42" spans="1:6" ht="11.25" customHeight="1">
       <c r="A42" s="13" t="s">
         <v>142</v>
       </c>
@@ -2516,7 +2896,7 @@
         <v>145</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="43">
+    <row r="43" spans="1:6" ht="10.15" customHeight="1">
       <c r="A43" s="13" t="s">
         <v>146</v>
       </c>
@@ -2534,7 +2914,7 @@
         <v>149</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="44" s="29">
+    <row r="44" spans="1:6" s="29" customFormat="1" ht="10.15" customHeight="1">
       <c r="A44" s="36" t="s">
         <v>150</v>
       </c>
@@ -2550,7 +2930,7 @@
         <v>153</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="45">
+    <row r="45" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A45" s="13" t="s">
         <v>154</v>
       </c>
@@ -2568,7 +2948,7 @@
         <v>158</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="46">
+    <row r="46" spans="1:6" ht="10.15" customHeight="1">
       <c r="A46" s="30" t="s">
         <v>159</v>
       </c>
@@ -2578,7 +2958,7 @@
       <c r="E46" s="30"/>
       <c r="F46" s="39"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="47" s="29">
+    <row r="47" spans="1:6" s="29" customFormat="1" ht="10.15" customHeight="1">
       <c r="A47" s="36" t="s">
         <v>160</v>
       </c>
@@ -2588,7 +2968,7 @@
       <c r="E47" s="36"/>
       <c r="F47" s="40"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="48" s="29">
+    <row r="48" spans="1:6" s="29" customFormat="1" ht="10.15" customHeight="1">
       <c r="A48" s="36" t="s">
         <v>161</v>
       </c>
@@ -2598,7 +2978,7 @@
       <c r="E48" s="36"/>
       <c r="F48" s="36"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="49">
+    <row r="49" spans="1:6" ht="10.15" customHeight="1">
       <c r="A49" s="30" t="s">
         <v>162</v>
       </c>
@@ -2608,7 +2988,7 @@
       <c r="E49" s="30"/>
       <c r="F49" s="39"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="50">
+    <row r="50" spans="1:6" ht="10.15" customHeight="1">
       <c r="A50" s="13" t="s">
         <v>163</v>
       </c>
@@ -2628,7 +3008,7 @@
         <v>166</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="51">
+    <row r="51" spans="1:6" ht="10.15" customHeight="1">
       <c r="A51" s="13" t="s">
         <v>167</v>
       </c>
@@ -2648,7 +3028,7 @@
         <v>170</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="52">
+    <row r="52" spans="1:6" ht="10.15" customHeight="1">
       <c r="A52" s="13" t="s">
         <v>171</v>
       </c>
@@ -2666,7 +3046,7 @@
         <v>173</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="53">
+    <row r="53" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A53" s="13" t="s">
         <v>174</v>
       </c>
@@ -2684,7 +3064,7 @@
         <v>176</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="54">
+    <row r="54" spans="1:6" ht="10.15" customHeight="1">
       <c r="A54" s="13" t="s">
         <v>177</v>
       </c>
@@ -2702,7 +3082,7 @@
         <v>180</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="55">
+    <row r="55" spans="1:6" ht="10.15" customHeight="1">
       <c r="A55" s="13" t="s">
         <v>181</v>
       </c>
@@ -2720,7 +3100,7 @@
         <v>184</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="56">
+    <row r="56" spans="1:6" ht="10.15" customHeight="1">
       <c r="A56" s="13" t="s">
         <v>185</v>
       </c>
@@ -2738,7 +3118,7 @@
         <v>187</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="57">
+    <row r="57" spans="1:6" ht="10.15" customHeight="1">
       <c r="A57" s="13" t="s">
         <v>188</v>
       </c>
@@ -2756,7 +3136,7 @@
         <v>190</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="58">
+    <row r="58" spans="1:6" ht="10.15" customHeight="1">
       <c r="A58" s="30" t="s">
         <v>191</v>
       </c>
@@ -2766,7 +3146,7 @@
       <c r="E58" s="30"/>
       <c r="F58" s="39"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="59">
+    <row r="59" spans="1:6" ht="10.15" customHeight="1">
       <c r="A59" s="13" t="s">
         <v>192</v>
       </c>
@@ -2786,7 +3166,7 @@
         <v>195</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="60">
+    <row r="60" spans="1:6" ht="10.15" customHeight="1">
       <c r="A60" s="13" t="s">
         <v>196</v>
       </c>
@@ -2806,7 +3186,7 @@
         <v>199</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="61">
+    <row r="61" spans="1:6" ht="10.15" customHeight="1">
       <c r="A61" s="13" t="s">
         <v>200</v>
       </c>
@@ -2824,7 +3204,7 @@
         <v>202</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="62">
+    <row r="62" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A62" s="13" t="s">
         <v>203</v>
       </c>
@@ -2842,7 +3222,7 @@
         <v>205</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="63">
+    <row r="63" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A63" s="13" t="s">
         <v>206</v>
       </c>
@@ -2860,7 +3240,7 @@
         <v>208</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="64">
+    <row r="64" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A64" s="13" t="s">
         <v>209</v>
       </c>
@@ -2878,7 +3258,7 @@
         <v>212</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="65">
+    <row r="65" spans="1:6" ht="10.15" customHeight="1">
       <c r="A65" s="30" t="s">
         <v>213</v>
       </c>
@@ -2888,7 +3268,7 @@
       <c r="E65" s="30"/>
       <c r="F65" s="39"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="66">
+    <row r="66" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A66" s="13" t="s">
         <v>214</v>
       </c>
@@ -2906,7 +3286,7 @@
         <v>217</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="67">
+    <row r="67" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A67" s="13" t="s">
         <v>218</v>
       </c>
@@ -2924,7 +3304,7 @@
         <v>220</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="68">
+    <row r="68" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A68" s="13" t="s">
         <v>221</v>
       </c>
@@ -2942,7 +3322,7 @@
         <v>224</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="69">
+    <row r="69" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A69" s="13" t="s">
         <v>225</v>
       </c>
@@ -2960,7 +3340,7 @@
         <v>228</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="70">
+    <row r="70" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A70" s="13" t="s">
         <v>229</v>
       </c>
@@ -2978,7 +3358,7 @@
         <v>231</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.1" outlineLevel="0" r="71">
+    <row r="71" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A71" s="13" t="s">
         <v>232</v>
       </c>
@@ -2996,7 +3376,7 @@
         <v>234</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="72">
+    <row r="72" spans="1:6" ht="10.15" customHeight="1">
       <c r="A72" s="30" t="s">
         <v>235</v>
       </c>
@@ -3006,7 +3386,7 @@
       <c r="E72" s="30"/>
       <c r="F72" s="39"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="73" s="44">
+    <row r="73" spans="1:6" s="44" customFormat="1" ht="10.15" customHeight="1">
       <c r="A73" s="41" t="s">
         <v>236</v>
       </c>
@@ -3022,7 +3402,7 @@
       <c r="E73" s="41"/>
       <c r="F73" s="41"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="74">
+    <row r="74" spans="1:6" ht="10.15" customHeight="1">
       <c r="A74" s="13" t="s">
         <v>239</v>
       </c>
@@ -3038,7 +3418,7 @@
       <c r="E74" s="13"/>
       <c r="F74" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="75">
+    <row r="75" spans="1:6" ht="10.15" customHeight="1">
       <c r="A75" s="13" t="s">
         <v>242</v>
       </c>
@@ -3054,7 +3434,7 @@
       <c r="E75" s="13"/>
       <c r="F75" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="76">
+    <row r="76" spans="1:6" ht="10.15" customHeight="1">
       <c r="A76" s="13" t="s">
         <v>245</v>
       </c>
@@ -3070,7 +3450,7 @@
       <c r="E76" s="13"/>
       <c r="F76" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="77">
+    <row r="77" spans="1:6" ht="10.15" customHeight="1">
       <c r="A77" s="13" t="s">
         <v>247</v>
       </c>
@@ -3086,7 +3466,7 @@
       <c r="E77" s="13"/>
       <c r="F77" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="78">
+    <row r="78" spans="1:6" ht="10.15" customHeight="1">
       <c r="A78" s="13" t="s">
         <v>249</v>
       </c>
@@ -3102,7 +3482,7 @@
       <c r="E78" s="13"/>
       <c r="F78" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="79">
+    <row r="79" spans="1:6" ht="10.15" customHeight="1">
       <c r="A79" s="13" t="s">
         <v>252</v>
       </c>
@@ -3118,7 +3498,7 @@
       <c r="E79" s="13"/>
       <c r="F79" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="80">
+    <row r="80" spans="1:6" ht="10.15" customHeight="1">
       <c r="A80" s="30" t="s">
         <v>254</v>
       </c>
@@ -3128,7 +3508,7 @@
       <c r="E80" s="30"/>
       <c r="F80" s="39"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="81">
+    <row r="81" spans="1:6" ht="10.15" customHeight="1">
       <c r="A81" s="13" t="s">
         <v>255</v>
       </c>
@@ -3144,7 +3524,7 @@
       <c r="E81" s="13"/>
       <c r="F81" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="82">
+    <row r="82" spans="1:6" ht="10.15" customHeight="1">
       <c r="A82" s="13" t="s">
         <v>258</v>
       </c>
@@ -3160,7 +3540,7 @@
       <c r="E82" s="13"/>
       <c r="F82" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="83">
+    <row r="83" spans="1:6" ht="10.15" customHeight="1">
       <c r="A83" s="30" t="s">
         <v>261</v>
       </c>
@@ -3170,7 +3550,7 @@
       <c r="E83" s="30"/>
       <c r="F83" s="39"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="84">
+    <row r="84" spans="1:6" ht="10.15" customHeight="1">
       <c r="A84" s="13" t="s">
         <v>262</v>
       </c>
@@ -3186,7 +3566,7 @@
       <c r="E84" s="13"/>
       <c r="F84" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="85">
+    <row r="85" spans="1:6" ht="10.15" customHeight="1">
       <c r="A85" s="30" t="s">
         <v>265</v>
       </c>
@@ -3196,7 +3576,7 @@
       <c r="E85" s="30"/>
       <c r="F85" s="39"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="86">
+    <row r="86" spans="1:6" ht="10.15" customHeight="1">
       <c r="A86" s="13" t="s">
         <v>266</v>
       </c>
@@ -3212,7 +3592,7 @@
       <c r="E86" s="13"/>
       <c r="F86" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="87">
+    <row r="87" spans="1:6" ht="10.15" customHeight="1">
       <c r="A87" s="13" t="s">
         <v>269</v>
       </c>
@@ -3228,7 +3608,7 @@
       <c r="E87" s="13"/>
       <c r="F87" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="88">
+    <row r="88" spans="1:6" ht="10.15" customHeight="1">
       <c r="A88" s="13" t="s">
         <v>272</v>
       </c>
@@ -3244,7 +3624,7 @@
       <c r="E88" s="13"/>
       <c r="F88" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="89">
+    <row r="89" spans="1:6" ht="10.15" customHeight="1">
       <c r="A89" s="13" t="s">
         <v>274</v>
       </c>
@@ -3260,7 +3640,7 @@
       <c r="E89" s="13"/>
       <c r="F89" s="35"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.1" outlineLevel="0" r="90">
+    <row r="90" spans="1:6" ht="10.15" customHeight="1">
       <c r="A90" s="13" t="s">
         <v>276</v>
       </c>
@@ -3277,36 +3657,29 @@
       <c r="F90" s="35"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2:D73"/>
+    <sheetView topLeftCell="A16" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D73"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3882352941176"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.6235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="85.8196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="26.3019607843137"/>
+    <col min="1" max="1" width="22.375"/>
+    <col min="2" max="2" width="36.625"/>
+    <col min="3" max="3" width="85.875"/>
+    <col min="4" max="4" width="25.125"/>
+    <col min="5" max="1025" width="26.25"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="1">
+    <row r="1" spans="1:4" ht="13.35" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3320,7 +3693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:4" ht="13.35" customHeight="1">
       <c r="A2" s="45" t="s">
         <v>6</v>
       </c>
@@ -3334,7 +3707,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" spans="1:4" ht="13.35" customHeight="1">
       <c r="A3" s="45" t="s">
         <v>11</v>
       </c>
@@ -3348,7 +3721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row r="4" spans="1:4" ht="13.35" customHeight="1">
       <c r="A4" s="45" t="s">
         <v>15</v>
       </c>
@@ -3362,7 +3735,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="5">
+    <row r="5" spans="1:4" ht="13.35" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
@@ -3376,7 +3749,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="6">
+    <row r="6" spans="1:4" ht="13.35" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
@@ -3390,7 +3763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="7">
+    <row r="7" spans="1:4" ht="13.35" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>27</v>
       </c>
@@ -3404,7 +3777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="8">
+    <row r="8" spans="1:4" ht="13.35" customHeight="1">
       <c r="A8" s="49" t="s">
         <v>31</v>
       </c>
@@ -3418,7 +3791,7 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="9">
+    <row r="9" spans="1:4" ht="13.35" customHeight="1">
       <c r="A9" s="49" t="s">
         <v>34</v>
       </c>
@@ -3432,7 +3805,7 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="10">
+    <row r="10" spans="1:4" ht="13.35" customHeight="1">
       <c r="A10" s="52" t="s">
         <v>37</v>
       </c>
@@ -3446,7 +3819,7 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="11">
+    <row r="11" spans="1:4" ht="13.35" customHeight="1">
       <c r="A11" s="11" t="s">
         <v>43</v>
       </c>
@@ -3460,7 +3833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="12">
+    <row r="12" spans="1:4" ht="13.35" customHeight="1">
       <c r="A12" s="11" t="s">
         <v>49</v>
       </c>
@@ -3474,7 +3847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="13">
+    <row r="13" spans="1:4" ht="13.35" customHeight="1">
       <c r="A13" s="11" t="s">
         <v>53</v>
       </c>
@@ -3488,7 +3861,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="14">
+    <row r="14" spans="1:4" ht="13.35" customHeight="1">
       <c r="A14" s="11" t="s">
         <v>58</v>
       </c>
@@ -3502,7 +3875,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="15">
+    <row r="15" spans="1:4" ht="13.35" customHeight="1">
       <c r="A15" s="11" t="s">
         <v>61</v>
       </c>
@@ -3516,7 +3889,7 @@
         <v>64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="16">
+    <row r="16" spans="1:4" ht="13.35" customHeight="1">
       <c r="A16" s="11" t="s">
         <v>66</v>
       </c>
@@ -3530,7 +3903,7 @@
         <v>64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="17">
+    <row r="17" spans="1:4" ht="13.35" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>69</v>
       </c>
@@ -3544,7 +3917,7 @@
         <v>64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="18">
+    <row r="18" spans="1:4" ht="13.35" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>72</v>
       </c>
@@ -3558,7 +3931,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="19">
+    <row r="19" spans="1:4" ht="13.35" customHeight="1">
       <c r="A19" s="11" t="s">
         <v>75</v>
       </c>
@@ -3572,7 +3945,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="20">
+    <row r="20" spans="1:4" ht="13.35" customHeight="1">
       <c r="A20" s="11" t="s">
         <v>79</v>
       </c>
@@ -3586,7 +3959,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="21">
+    <row r="21" spans="1:4" ht="13.35" customHeight="1">
       <c r="A21" s="11" t="s">
         <v>82</v>
       </c>
@@ -3600,7 +3973,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="22">
+    <row r="22" spans="1:4" ht="13.35" customHeight="1">
       <c r="A22" s="11" t="s">
         <v>86</v>
       </c>
@@ -3614,7 +3987,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="23">
+    <row r="23" spans="1:4" ht="13.35" customHeight="1">
       <c r="A23" s="11" t="s">
         <v>90</v>
       </c>
@@ -3628,7 +4001,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="24">
+    <row r="24" spans="1:4" ht="13.35" customHeight="1">
       <c r="A24" s="11" t="s">
         <v>94</v>
       </c>
@@ -3642,7 +4015,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="25">
+    <row r="25" spans="1:4" ht="13.35" customHeight="1">
       <c r="A25" s="11" t="s">
         <v>98</v>
       </c>
@@ -3656,7 +4029,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="26">
+    <row r="26" spans="1:4" ht="13.35" customHeight="1">
       <c r="A26" s="11" t="s">
         <v>101</v>
       </c>
@@ -3670,7 +4043,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="27">
+    <row r="27" spans="1:4" ht="13.35" customHeight="1">
       <c r="A27" s="11" t="s">
         <v>104</v>
       </c>
@@ -3684,7 +4057,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="28">
+    <row r="28" spans="1:4" ht="13.35" customHeight="1">
       <c r="A28" s="11" t="s">
         <v>108</v>
       </c>
@@ -3698,7 +4071,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="29">
+    <row r="29" spans="1:4" ht="13.35" customHeight="1">
       <c r="A29" s="11" t="s">
         <v>112</v>
       </c>
@@ -3712,7 +4085,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="30">
+    <row r="30" spans="1:4" ht="13.35" customHeight="1">
       <c r="A30" s="11" t="s">
         <v>115</v>
       </c>
@@ -3726,7 +4099,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="31">
+    <row r="31" spans="1:4" ht="13.35" customHeight="1">
       <c r="A31" s="34" t="s">
         <v>118</v>
       </c>
@@ -3740,7 +4113,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="32">
+    <row r="32" spans="1:4" ht="13.35" customHeight="1">
       <c r="A32" s="11" t="s">
         <v>121</v>
       </c>
@@ -3754,7 +4127,7 @@
         <v>123</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="33">
+    <row r="33" spans="1:4" ht="13.35" customHeight="1">
       <c r="A33" s="11" t="s">
         <v>125</v>
       </c>
@@ -3768,7 +4141,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="34">
+    <row r="34" spans="1:4" ht="13.35" customHeight="1">
       <c r="A34" s="11" t="s">
         <v>128</v>
       </c>
@@ -3782,7 +4155,7 @@
         <v>130</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="35">
+    <row r="35" spans="1:4" ht="13.35" customHeight="1">
       <c r="A35" s="11" t="s">
         <v>132</v>
       </c>
@@ -3796,7 +4169,7 @@
         <v>135</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="36">
+    <row r="36" spans="1:4" ht="13.35" customHeight="1">
       <c r="A36" s="11" t="s">
         <v>137</v>
       </c>
@@ -3810,7 +4183,7 @@
         <v>140</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="37">
+    <row r="37" spans="1:4" ht="13.35" customHeight="1">
       <c r="A37" s="11" t="s">
         <v>142</v>
       </c>
@@ -3824,7 +4197,7 @@
         <v>140</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="38">
+    <row r="38" spans="1:4" ht="13.35" customHeight="1">
       <c r="A38" s="11" t="s">
         <v>146</v>
       </c>
@@ -3838,7 +4211,7 @@
         <v>140</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="39">
+    <row r="39" spans="1:4" ht="13.35" customHeight="1">
       <c r="A39" s="11" t="s">
         <v>154</v>
       </c>
@@ -3852,7 +4225,7 @@
         <v>157</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="40">
+    <row r="40" spans="1:4" ht="13.35" customHeight="1">
       <c r="A40" s="11" t="s">
         <v>163</v>
       </c>
@@ -3866,7 +4239,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="41">
+    <row r="41" spans="1:4" ht="13.35" customHeight="1">
       <c r="A41" s="11" t="s">
         <v>167</v>
       </c>
@@ -3880,7 +4253,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="42">
+    <row r="42" spans="1:4" ht="13.35" customHeight="1">
       <c r="A42" s="11" t="s">
         <v>171</v>
       </c>
@@ -3894,7 +4267,7 @@
         <v>157</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="43">
+    <row r="43" spans="1:4" ht="13.35" customHeight="1">
       <c r="A43" s="11" t="s">
         <v>174</v>
       </c>
@@ -3908,7 +4281,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="44">
+    <row r="44" spans="1:4" ht="13.35" customHeight="1">
       <c r="A44" s="11" t="s">
         <v>177</v>
       </c>
@@ -3922,7 +4295,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="45">
+    <row r="45" spans="1:4" ht="13.35" customHeight="1">
       <c r="A45" s="11" t="s">
         <v>181</v>
       </c>
@@ -3936,7 +4309,7 @@
         <v>157</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="46">
+    <row r="46" spans="1:4" ht="13.35" customHeight="1">
       <c r="A46" s="11" t="s">
         <v>185</v>
       </c>
@@ -3950,7 +4323,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="47">
+    <row r="47" spans="1:4" ht="13.35" customHeight="1">
       <c r="A47" s="11" t="s">
         <v>188</v>
       </c>
@@ -3964,7 +4337,7 @@
         <v>157</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="48">
+    <row r="48" spans="1:4" ht="13.35" customHeight="1">
       <c r="A48" s="11" t="s">
         <v>192</v>
       </c>
@@ -3978,7 +4351,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="49">
+    <row r="49" spans="1:4" ht="13.35" customHeight="1">
       <c r="A49" s="11" t="s">
         <v>196</v>
       </c>
@@ -3992,7 +4365,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="50">
+    <row r="50" spans="1:4" ht="13.35" customHeight="1">
       <c r="A50" s="11" t="s">
         <v>200</v>
       </c>
@@ -4006,7 +4379,7 @@
         <v>157</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="51">
+    <row r="51" spans="1:4" ht="13.35" customHeight="1">
       <c r="A51" s="11" t="s">
         <v>203</v>
       </c>
@@ -4020,7 +4393,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="52">
+    <row r="52" spans="1:4" ht="13.35" customHeight="1">
       <c r="A52" s="11" t="s">
         <v>206</v>
       </c>
@@ -4034,7 +4407,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="53">
+    <row r="53" spans="1:4" ht="13.35" customHeight="1">
       <c r="A53" s="11" t="s">
         <v>209</v>
       </c>
@@ -4048,7 +4421,7 @@
         <v>157</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="54">
+    <row r="54" spans="1:4" ht="13.35" customHeight="1">
       <c r="A54" s="11" t="s">
         <v>214</v>
       </c>
@@ -4062,7 +4435,7 @@
         <v>157</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="55">
+    <row r="55" spans="1:4" ht="13.35" customHeight="1">
       <c r="A55" s="11" t="s">
         <v>218</v>
       </c>
@@ -4076,7 +4449,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="56">
+    <row r="56" spans="1:4" ht="13.35" customHeight="1">
       <c r="A56" s="11" t="s">
         <v>221</v>
       </c>
@@ -4090,7 +4463,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="57">
+    <row r="57" spans="1:4" ht="13.35" customHeight="1">
       <c r="A57" s="11" t="s">
         <v>225</v>
       </c>
@@ -4104,7 +4477,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="58">
+    <row r="58" spans="1:4" ht="13.35" customHeight="1">
       <c r="A58" s="11" t="s">
         <v>229</v>
       </c>
@@ -4118,7 +4491,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="59">
+    <row r="59" spans="1:4" ht="13.35" customHeight="1">
       <c r="A59" s="11" t="s">
         <v>232</v>
       </c>
@@ -4132,7 +4505,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="60">
+    <row r="60" spans="1:4" ht="13.35" customHeight="1">
       <c r="A60" s="11" t="s">
         <v>239</v>
       </c>
@@ -4146,7 +4519,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="61">
+    <row r="61" spans="1:4" ht="13.35" customHeight="1">
       <c r="A61" s="11" t="s">
         <v>242</v>
       </c>
@@ -4160,7 +4533,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="62">
+    <row r="62" spans="1:4" ht="13.35" customHeight="1">
       <c r="A62" s="11" t="s">
         <v>245</v>
       </c>
@@ -4174,7 +4547,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="63">
+    <row r="63" spans="1:4" ht="13.35" customHeight="1">
       <c r="A63" s="11" t="s">
         <v>247</v>
       </c>
@@ -4188,7 +4561,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="64">
+    <row r="64" spans="1:4" ht="13.35" customHeight="1">
       <c r="A64" s="11" t="s">
         <v>249</v>
       </c>
@@ -4202,7 +4575,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="65">
+    <row r="65" spans="1:4" ht="13.35" customHeight="1">
       <c r="A65" s="11" t="s">
         <v>252</v>
       </c>
@@ -4216,7 +4589,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="66">
+    <row r="66" spans="1:4" ht="13.35" customHeight="1">
       <c r="A66" s="11" t="s">
         <v>255</v>
       </c>
@@ -4230,7 +4603,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="67">
+    <row r="67" spans="1:4" ht="13.35" customHeight="1">
       <c r="A67" s="11" t="s">
         <v>258</v>
       </c>
@@ -4244,7 +4617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="68">
+    <row r="68" spans="1:4" ht="13.35" customHeight="1">
       <c r="A68" s="11" t="s">
         <v>262</v>
       </c>
@@ -4258,7 +4631,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="69">
+    <row r="69" spans="1:4" ht="13.35" customHeight="1">
       <c r="A69" s="11" t="s">
         <v>266</v>
       </c>
@@ -4272,7 +4645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="70">
+    <row r="70" spans="1:4" ht="13.35" customHeight="1">
       <c r="A70" s="11" t="s">
         <v>269</v>
       </c>
@@ -4286,7 +4659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="71">
+    <row r="71" spans="1:4" ht="13.35" customHeight="1">
       <c r="A71" s="11" t="s">
         <v>272</v>
       </c>
@@ -4300,7 +4673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="72">
+    <row r="72" spans="1:4" ht="13.35" customHeight="1">
       <c r="A72" s="11" t="s">
         <v>274</v>
       </c>
@@ -4314,7 +4687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="73">
+    <row r="73" spans="1:4" ht="13.35" customHeight="1">
       <c r="A73" s="11" t="s">
         <v>276</v>
       </c>
@@ -4329,40 +4702,33 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:AMK25"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F27" activeCellId="1" pane="topLeft" sqref="B2:D73 F27"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" activeCellId="1" sqref="B2:D73 F27"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="56" width="11.1921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="56" width="16.3647058823529"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="56" width="16.1921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="56" width="9.12941176470588"/>
+    <col min="1" max="1" width="11.25" style="56"/>
+    <col min="2" max="2" width="16.375" style="56"/>
+    <col min="3" max="3" width="16.25" style="56"/>
+    <col min="4" max="1025" width="9.125" style="56"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.5" outlineLevel="0" r="1" s="58">
+    <row r="1" spans="1:3" s="58" customFormat="1" ht="19.5" customHeight="1">
       <c r="A1" s="57" t="s">
         <v>278</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.25" outlineLevel="0" r="2">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1">
       <c r="A2" s="59" t="s">
         <v>279</v>
       </c>
@@ -4373,8 +4739,8 @@
         <v>281</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.25" outlineLevel="0" r="3">
-      <c r="A3" s="60" t="s">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1">
+      <c r="A3" s="73" t="s">
         <v>282</v>
       </c>
       <c r="B3" s="61" t="s">
@@ -4384,224 +4750,217 @@
         <v>284</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.25" outlineLevel="0" r="4">
-      <c r="A4" s="60"/>
+    <row r="4" spans="1:3" ht="17.25" customHeight="1">
+      <c r="A4" s="73"/>
       <c r="B4" s="61" t="s">
         <v>285</v>
       </c>
       <c r="C4" s="61"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="5">
-      <c r="A5" s="62" t="s">
+    <row r="5" spans="1:3" ht="12" customHeight="1">
+      <c r="A5" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="62" t="s">
         <v>287</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="63" t="s">
         <v>288</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="6">
-      <c r="A6" s="62"/>
-      <c r="B6" s="63" t="s">
+    <row r="6" spans="1:3" ht="12" customHeight="1">
+      <c r="A6" s="72"/>
+      <c r="B6" s="62" t="s">
         <v>289</v>
       </c>
-      <c r="C6" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="7">
-      <c r="A7" s="62" t="s">
+      <c r="C6" s="63"/>
+    </row>
+    <row r="7" spans="1:3" ht="12" customHeight="1">
+      <c r="A7" s="72" t="s">
         <v>290</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="62" t="s">
         <v>291</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="63" t="s">
         <v>292</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="8">
-      <c r="A8" s="62"/>
-      <c r="B8" s="63" t="s">
+    <row r="8" spans="1:3" ht="12" customHeight="1">
+      <c r="A8" s="72"/>
+      <c r="B8" s="62" t="s">
         <v>293</v>
       </c>
-      <c r="C8" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="9">
-      <c r="A9" s="62"/>
-      <c r="B9" s="63" t="s">
+      <c r="C8" s="63"/>
+    </row>
+    <row r="9" spans="1:3" ht="12" customHeight="1">
+      <c r="A9" s="72"/>
+      <c r="B9" s="62" t="s">
         <v>294</v>
       </c>
-      <c r="C9" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="10">
-      <c r="A10" s="62"/>
-      <c r="B10" s="63" t="s">
+      <c r="C9" s="63"/>
+    </row>
+    <row r="10" spans="1:3" ht="12" customHeight="1">
+      <c r="A10" s="72"/>
+      <c r="B10" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="C10" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="11">
-      <c r="A11" s="62" t="s">
+      <c r="C10" s="63"/>
+    </row>
+    <row r="11" spans="1:3" ht="12" customHeight="1">
+      <c r="A11" s="72" t="s">
         <v>296</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="62" t="s">
         <v>297</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="63" t="s">
         <v>298</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="12">
-      <c r="A12" s="62"/>
-      <c r="B12" s="63" t="s">
+    <row r="12" spans="1:3" ht="12" customHeight="1">
+      <c r="A12" s="72"/>
+      <c r="B12" s="62" t="s">
         <v>291</v>
       </c>
-      <c r="C12" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="13">
-      <c r="A13" s="62"/>
-      <c r="B13" s="63" t="s">
+      <c r="C12" s="63"/>
+    </row>
+    <row r="13" spans="1:3" ht="12" customHeight="1">
+      <c r="A13" s="72"/>
+      <c r="B13" s="62" t="s">
         <v>293</v>
       </c>
-      <c r="C13" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="14">
-      <c r="A14" s="62"/>
-      <c r="B14" s="63" t="s">
+      <c r="C13" s="63"/>
+    </row>
+    <row r="14" spans="1:3" ht="12" customHeight="1">
+      <c r="A14" s="72"/>
+      <c r="B14" s="62" t="s">
         <v>294</v>
       </c>
-      <c r="C14" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="15">
-      <c r="A15" s="62"/>
-      <c r="B15" s="63" t="s">
+      <c r="C14" s="63"/>
+    </row>
+    <row r="15" spans="1:3" ht="12" customHeight="1">
+      <c r="A15" s="72"/>
+      <c r="B15" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="C15" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="16">
-      <c r="A16" s="62" t="s">
+      <c r="C15" s="63"/>
+    </row>
+    <row r="16" spans="1:3" ht="12" customHeight="1">
+      <c r="A16" s="72" t="s">
         <v>299</v>
       </c>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="62" t="s">
         <v>297</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="63" t="s">
         <v>300</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="17">
-      <c r="A17" s="62"/>
-      <c r="B17" s="63" t="s">
+    <row r="17" spans="1:3" ht="12" customHeight="1">
+      <c r="A17" s="72"/>
+      <c r="B17" s="62" t="s">
         <v>291</v>
       </c>
-      <c r="C17" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="18">
-      <c r="A18" s="62"/>
-      <c r="B18" s="63" t="s">
+      <c r="C17" s="63"/>
+    </row>
+    <row r="18" spans="1:3" ht="12" customHeight="1">
+      <c r="A18" s="72"/>
+      <c r="B18" s="62" t="s">
         <v>293</v>
       </c>
-      <c r="C18" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="19">
-      <c r="A19" s="62"/>
-      <c r="B19" s="63" t="s">
+      <c r="C18" s="63"/>
+    </row>
+    <row r="19" spans="1:3" ht="12" customHeight="1">
+      <c r="A19" s="72"/>
+      <c r="B19" s="62" t="s">
         <v>301</v>
       </c>
-      <c r="C19" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="20">
-      <c r="A20" s="62"/>
-      <c r="B20" s="63" t="s">
+      <c r="C19" s="63"/>
+    </row>
+    <row r="20" spans="1:3" ht="12" customHeight="1">
+      <c r="A20" s="72"/>
+      <c r="B20" s="62" t="s">
         <v>302</v>
       </c>
-      <c r="C20" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="21">
-      <c r="A21" s="62" t="s">
+      <c r="C20" s="63"/>
+    </row>
+    <row r="21" spans="1:3" ht="12" customHeight="1">
+      <c r="A21" s="72" t="s">
         <v>303</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="62" t="s">
         <v>297</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="63" t="s">
         <v>304</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="22">
-      <c r="A22" s="62"/>
-      <c r="B22" s="63" t="s">
+    <row r="22" spans="1:3" ht="12" customHeight="1">
+      <c r="A22" s="72"/>
+      <c r="B22" s="62" t="s">
         <v>291</v>
       </c>
-      <c r="C22" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="23">
-      <c r="A23" s="62"/>
-      <c r="B23" s="63" t="s">
+      <c r="C22" s="63"/>
+    </row>
+    <row r="23" spans="1:3" ht="12" customHeight="1">
+      <c r="A23" s="72"/>
+      <c r="B23" s="62" t="s">
         <v>293</v>
       </c>
-      <c r="C23" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="24">
-      <c r="A24" s="62"/>
-      <c r="B24" s="63" t="s">
+      <c r="C23" s="63"/>
+    </row>
+    <row r="24" spans="1:3" ht="12" customHeight="1">
+      <c r="A24" s="72"/>
+      <c r="B24" s="62" t="s">
         <v>305</v>
       </c>
-      <c r="C24" s="64"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="25">
-      <c r="A25" s="62"/>
-      <c r="B25" s="63" t="s">
+      <c r="C24" s="63"/>
+    </row>
+    <row r="25" spans="1:3" ht="12" customHeight="1">
+      <c r="A25" s="72"/>
+      <c r="B25" s="62" t="s">
         <v>306</v>
       </c>
-      <c r="C25" s="64"/>
+      <c r="C25" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A21:A25"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A15"/>
     <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A21:A25"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:AMK16"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H20" activeCellId="1" pane="topLeft" sqref="B2:D73 H20"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" activeCellId="1" sqref="A2:D73 H20"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="65" width="11.1921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="65" width="39.2901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="65" width="9.12941176470588"/>
+    <col min="1" max="1" width="11.25" style="64"/>
+    <col min="2" max="2" width="39.25" style="64"/>
+    <col min="3" max="1025" width="9.125" style="64"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="1" s="67">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:2" s="65" customFormat="1" ht="14.1" customHeight="1">
+      <c r="A1" s="74" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="66"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="2">
+      <c r="B1" s="74"/>
+    </row>
+    <row r="2" spans="1:2" ht="14.1" customHeight="1">
       <c r="A2" s="59" t="s">
         <v>279</v>
       </c>
@@ -4609,7 +4968,7 @@
         <v>281</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="3">
+    <row r="3" spans="1:2" ht="14.1" customHeight="1">
       <c r="A3" s="60" t="s">
         <v>282</v>
       </c>
@@ -4617,77 +4976,77 @@
         <v>284</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="4">
-      <c r="A4" s="68" t="s">
+    <row r="4" spans="1:2" ht="14.1" customHeight="1">
+      <c r="A4" s="66" t="s">
         <v>286</v>
       </c>
       <c r="B4" s="61" t="s">
         <v>308</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="5">
-      <c r="A5" s="68" t="s">
+    <row r="5" spans="1:2" ht="14.1" customHeight="1">
+      <c r="A5" s="66" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="61" t="s">
         <v>309</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="6">
-      <c r="A6" s="68" t="s">
+    <row r="6" spans="1:2" ht="14.1" customHeight="1">
+      <c r="A6" s="66" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="61" t="s">
         <v>292</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="7">
-      <c r="A7" s="68" t="s">
+    <row r="7" spans="1:2" ht="14.1" customHeight="1">
+      <c r="A7" s="66" t="s">
         <v>296</v>
       </c>
       <c r="B7" s="61" t="s">
         <v>310</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="8">
-      <c r="A8" s="68" t="s">
+    <row r="8" spans="1:2" ht="14.1" customHeight="1">
+      <c r="A8" s="66" t="s">
         <v>299</v>
       </c>
       <c r="B8" s="61" t="s">
         <v>300</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="9">
-      <c r="A9" s="68" t="s">
+    <row r="9" spans="1:2" ht="14.1" customHeight="1">
+      <c r="A9" s="66" t="s">
         <v>303</v>
       </c>
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="67" t="s">
         <v>304</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="10">
-      <c r="A10" s="68" t="s">
+    <row r="10" spans="1:2" ht="14.1" customHeight="1">
+      <c r="A10" s="66" t="s">
         <v>311</v>
       </c>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="67" t="s">
         <v>312</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="11">
-      <c r="A11" s="68" t="s">
+    <row r="11" spans="1:2" ht="14.1" customHeight="1">
+      <c r="A11" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="67" t="s">
         <v>313</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="13">
-      <c r="A13" s="66" t="s">
+    <row r="13" spans="1:2" ht="14.1" customHeight="1">
+      <c r="A13" s="74" t="s">
         <v>314</v>
       </c>
-      <c r="B13" s="66"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="14">
+      <c r="B13" s="74"/>
+    </row>
+    <row r="14" spans="1:2" ht="14.1" customHeight="1">
       <c r="A14" s="59" t="s">
         <v>279</v>
       </c>
@@ -4695,7 +5054,7 @@
         <v>281</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="15">
+    <row r="15" spans="1:2" ht="14.1" customHeight="1">
       <c r="A15" s="60" t="s">
         <v>14</v>
       </c>
@@ -4703,7 +5062,7 @@
         <v>315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23" outlineLevel="0" r="16">
+    <row r="16" spans="1:2" ht="23.1" customHeight="1">
       <c r="A16" s="60" t="s">
         <v>316</v>
       </c>
@@ -4716,12 +5075,331 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A13:B13"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8" style="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.75" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.25" style="71" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="69"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="68" customFormat="1">
+      <c r="A1" s="68" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>319</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>320</v>
+      </c>
+      <c r="D1" s="70" t="s">
+        <v>321</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>322</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="69" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="69" t="s">
+        <v>325</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>331</v>
+      </c>
+      <c r="F2" s="69" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="69" t="s">
+        <v>327</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3" s="71" t="s">
+        <v>332</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="69" t="s">
+        <v>329</v>
+      </c>
+      <c r="C4" s="69" t="s">
+        <v>330</v>
+      </c>
+      <c r="D4" s="71" t="s">
+        <v>333</v>
+      </c>
+      <c r="F4" s="69" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.75" style="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.375" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.25" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.875" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.75" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.625" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.25" style="69" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="69" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" style="69" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="69"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="68" customFormat="1">
+      <c r="A1" s="68" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>334</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>320</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>335</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>336</v>
+      </c>
+      <c r="G1" s="68" t="s">
+        <v>337</v>
+      </c>
+      <c r="H1" s="68" t="s">
+        <v>322</v>
+      </c>
+      <c r="I1" s="68" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="C2" s="69" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="69" t="s">
+        <v>339</v>
+      </c>
+      <c r="E2" s="69">
+        <v>100</v>
+      </c>
+      <c r="F2" s="69">
+        <v>310</v>
+      </c>
+      <c r="G2" s="69">
+        <v>480</v>
+      </c>
+      <c r="I2" s="69" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="C3" s="69" t="s">
+        <v>340</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>341</v>
+      </c>
+      <c r="E3" s="69">
+        <v>80</v>
+      </c>
+      <c r="F3" s="69">
+        <v>0</v>
+      </c>
+      <c r="G3" s="69">
+        <v>920</v>
+      </c>
+      <c r="I3" s="69" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="C4" s="69" t="s">
+        <v>342</v>
+      </c>
+      <c r="D4" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="E4" s="69">
+        <v>50</v>
+      </c>
+      <c r="F4" s="69">
+        <v>0</v>
+      </c>
+      <c r="G4" s="69">
+        <v>1480</v>
+      </c>
+      <c r="I4" s="69" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.25" style="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="69"/>
+    <col min="3" max="3" width="8.375" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.375" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.375" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.75" style="69" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="69" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="69" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.625" style="69" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.875" style="69" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.375" style="69" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="69"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>334</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>318</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>320</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>346</v>
+      </c>
+      <c r="G1" s="69" t="s">
+        <v>347</v>
+      </c>
+      <c r="H1" s="69" t="s">
+        <v>348</v>
+      </c>
+      <c r="I1" s="69" t="s">
+        <v>349</v>
+      </c>
+      <c r="J1" s="69" t="s">
+        <v>336</v>
+      </c>
+      <c r="K1" s="69" t="s">
+        <v>322</v>
+      </c>
+      <c r="L1" s="69" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="D2" s="69" t="s">
+        <v>350</v>
+      </c>
+      <c r="E2" s="69" t="s">
+        <v>351</v>
+      </c>
+      <c r="F2" s="69">
+        <v>480</v>
+      </c>
+      <c r="J2" s="69">
+        <v>0</v>
+      </c>
+      <c r="L2" s="69" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="D3" s="69" t="s">
+        <v>352</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>353</v>
+      </c>
+      <c r="F3" s="69">
+        <v>920</v>
+      </c>
+      <c r="J3" s="69">
+        <v>0</v>
+      </c>
+      <c r="L3" s="69" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="D4" s="69" t="s">
+        <v>354</v>
+      </c>
+      <c r="E4" s="69" t="s">
+        <v>355</v>
+      </c>
+      <c r="F4" s="69">
+        <v>1480</v>
+      </c>
+      <c r="J4" s="69">
+        <v>0</v>
+      </c>
+      <c r="L4" s="69" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>